<commit_message>
[Fixing tip calculation, relabeling Amount Charged to Total (Pre-Tip)
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,24 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jose\Documents\UiPath\UberReceipts\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E92D1D9C-DA42-4A49-8826-94C82C6CA25F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BED40047-83E2-449A-9494-CE13849BC910}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10546" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
     <sheet name="Constants" sheetId="2" r:id="rId2"/>
     <sheet name="Assets" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
-  <fileRecoveryPr repairLoad="1"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -205,10 +214,10 @@
     <t>Subject</t>
   </si>
   <si>
-    <t>Subject of the mail messages wanted for extraction</t>
-  </si>
-  <si>
     <t>Uber Receipts</t>
+  </si>
+  <si>
+    <t>Subject of the mail messages wanted for extraction (Now used for from name instead)</t>
   </si>
 </sst>
 </file>
@@ -568,8 +577,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z991"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.3984375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -671,7 +680,7 @@
         <v>55</v>
       </c>
       <c r="B7" s="2">
-        <v>43709</v>
+        <v>43879</v>
       </c>
       <c r="C7" t="s">
         <v>57</v>
@@ -682,7 +691,7 @@
         <v>56</v>
       </c>
       <c r="B8" s="2">
-        <v>43722</v>
+        <v>43882</v>
       </c>
       <c r="C8" t="s">
         <v>58</v>
@@ -693,10 +702,10 @@
         <v>59</v>
       </c>
       <c r="B9" t="s">
+        <v>60</v>
+      </c>
+      <c r="C9" t="s">
         <v>61</v>
-      </c>
-      <c r="C9" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>

</xml_diff>